<commit_message>
Cleaned up code for making videos
</commit_message>
<xml_diff>
--- a/Inputs/HighFreqLabels.xlsx
+++ b/Inputs/HighFreqLabels.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="168">
   <si>
     <t>Label</t>
   </si>
@@ -44,220 +44,490 @@
     <t>Timestep</t>
   </si>
   <si>
-    <t>Before Drug\HighFreq_4</t>
-  </si>
-  <si>
-    <t>Before Drug\HighFreq_5</t>
-  </si>
-  <si>
-    <t>Before Drug\HighFreq_6</t>
-  </si>
-  <si>
-    <t>Before Drug\HighFreq_7</t>
-  </si>
-  <si>
-    <t>Before Drug\HighFreq_8</t>
-  </si>
-  <si>
-    <t>Before Drug\HighFreq_9</t>
-  </si>
-  <si>
-    <t>Before Drug\HighFreq_10</t>
-  </si>
-  <si>
-    <t>Before Drug\HighFreq_11</t>
-  </si>
-  <si>
-    <t>Before Drug\HighFreq_12</t>
-  </si>
-  <si>
-    <t>Before Drug\HighFreq_13</t>
-  </si>
-  <si>
-    <t>Before Drug\HighFreq_14</t>
-  </si>
-  <si>
-    <t>Before Drug\HighFreq_15</t>
-  </si>
-  <si>
-    <t>Before Drug\HighFreq_16</t>
-  </si>
-  <si>
-    <t>Before Drug\HighFreq_17</t>
-  </si>
-  <si>
-    <t>Before Drug\HighFreq_18</t>
-  </si>
-  <si>
-    <t>Before Drug\HighFreq_19</t>
-  </si>
-  <si>
-    <t>Before Drug\HighFreq_20</t>
-  </si>
-  <si>
-    <t>Before Drug\HighFreq_21</t>
-  </si>
-  <si>
-    <t>After Drug\HighFreq_1</t>
-  </si>
-  <si>
-    <t>After Drug\HighFreq_2</t>
-  </si>
-  <si>
-    <t>After Drug\HighFreq_3</t>
-  </si>
-  <si>
-    <t>After Drug\HighFreq_4</t>
-  </si>
-  <si>
-    <t>After Drug\HighFreq_5</t>
-  </si>
-  <si>
-    <t>After Drug\HighFreq_6</t>
-  </si>
-  <si>
-    <t>After Drug\HighFreq_7</t>
-  </si>
-  <si>
-    <t>After Drug\HighFreq_8</t>
-  </si>
-  <si>
-    <t>After Drug\HighFreq_9</t>
-  </si>
-  <si>
-    <t>After Drug\HighFreq_10</t>
-  </si>
-  <si>
-    <t>After Drug\HighFreq_11</t>
-  </si>
-  <si>
-    <t>After Drug\HighFreq_12</t>
-  </si>
-  <si>
-    <t>After Drug\HighFreq_13</t>
-  </si>
-  <si>
-    <t>After Drug\HighFreq_14</t>
-  </si>
-  <si>
-    <t>After Drug\HighFreq_15</t>
-  </si>
-  <si>
-    <t>After Drug\HighFreq_16</t>
-  </si>
-  <si>
-    <t>After Drug\HighFreq_17</t>
-  </si>
-  <si>
-    <t>After Drug\HighFreq_18</t>
-  </si>
-  <si>
-    <t>After Drug\HighFreq_19</t>
-  </si>
-  <si>
-    <t>After Drug\HighFreq_20</t>
-  </si>
-  <si>
-    <t>After Drug\HighFreq_21</t>
-  </si>
-  <si>
-    <t>After Drug\HighFreq_22</t>
-  </si>
-  <si>
-    <t>After Drug\HighFreq_23</t>
-  </si>
-  <si>
-    <t>After Drug\HighFreq_24</t>
-  </si>
-  <si>
-    <t>After Drug\HighFreq_25</t>
-  </si>
-  <si>
-    <t>After Drug\HighFreq_26</t>
-  </si>
-  <si>
-    <t>After Drug\HighFreq_27</t>
-  </si>
-  <si>
-    <t>After Drug\HighFreq_28</t>
-  </si>
-  <si>
-    <t>After Drug\HighFreq_29</t>
-  </si>
-  <si>
-    <t>After Drug\HighFreq_30</t>
-  </si>
-  <si>
-    <t>After Drug\HighFreq_31</t>
-  </si>
-  <si>
-    <t>After Drug\HighFreq_32</t>
-  </si>
-  <si>
-    <t>After Drug\HighFreq_33</t>
-  </si>
-  <si>
-    <t>After Drug\HighFreq_34</t>
-  </si>
-  <si>
-    <t>After Drug\HighFreq_35</t>
-  </si>
-  <si>
-    <t>After Drug\HighFreq_36</t>
-  </si>
-  <si>
-    <t>After Drug\HighFreq_37</t>
-  </si>
-  <si>
-    <t>After Drug\HighFreq_38</t>
-  </si>
-  <si>
-    <t>After Drug\HighFreq_39</t>
-  </si>
-  <si>
-    <t>After Drug\HighFreq_40</t>
-  </si>
-  <si>
-    <t>After Drug\HighFreq_41</t>
-  </si>
-  <si>
-    <t>After Drug\HighFreq_42</t>
-  </si>
-  <si>
-    <t>After Drug\HighFreq_43</t>
-  </si>
-  <si>
-    <t>After Drug\HighFreq_44</t>
-  </si>
-  <si>
-    <t>After Drug\HighFreq_45</t>
-  </si>
-  <si>
-    <t>After Drug\HighFreq_46</t>
-  </si>
-  <si>
-    <t>After Drug\HighFreq_47</t>
-  </si>
-  <si>
-    <t>After Drug\HighFreq_48</t>
-  </si>
-  <si>
-    <t>After Drug\HighFreq_49</t>
-  </si>
-  <si>
     <t>Treated</t>
   </si>
   <si>
     <t>Media</t>
   </si>
   <si>
-    <t>ZO fort</t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
     <t>Days</t>
+  </si>
+  <si>
+    <t>Day1\Before Drug\HighFreq_4</t>
+  </si>
+  <si>
+    <t>Day1\Before Drug\HighFreq_5</t>
+  </si>
+  <si>
+    <t>Day1\Before Drug\HighFreq_6</t>
+  </si>
+  <si>
+    <t>Day1\Before Drug\HighFreq_7</t>
+  </si>
+  <si>
+    <t>Day1\Before Drug\HighFreq_8</t>
+  </si>
+  <si>
+    <t>Day1\Before Drug\HighFreq_9</t>
+  </si>
+  <si>
+    <t>Day1\Before Drug\HighFreq_10</t>
+  </si>
+  <si>
+    <t>Day1\Before Drug\HighFreq_11</t>
+  </si>
+  <si>
+    <t>Day1\Before Drug\HighFreq_12</t>
+  </si>
+  <si>
+    <t>Day1\Before Drug\HighFreq_13</t>
+  </si>
+  <si>
+    <t>Day1\Before Drug\HighFreq_14</t>
+  </si>
+  <si>
+    <t>Day1\Before Drug\HighFreq_15</t>
+  </si>
+  <si>
+    <t>Day1\Before Drug\HighFreq_16</t>
+  </si>
+  <si>
+    <t>Day1\Before Drug\HighFreq_17</t>
+  </si>
+  <si>
+    <t>Day1\Before Drug\HighFreq_18</t>
+  </si>
+  <si>
+    <t>Day1\Before Drug\HighFreq_19</t>
+  </si>
+  <si>
+    <t>Day1\Before Drug\HighFreq_20</t>
+  </si>
+  <si>
+    <t>Day1\Before Drug\HighFreq_21</t>
+  </si>
+  <si>
+    <t>Day1\After Drug\HighFreq_1</t>
+  </si>
+  <si>
+    <t>Day1\After Drug\HighFreq_2</t>
+  </si>
+  <si>
+    <t>Day1\After Drug\HighFreq_3</t>
+  </si>
+  <si>
+    <t>Day1\After Drug\HighFreq_4</t>
+  </si>
+  <si>
+    <t>Day1\After Drug\HighFreq_5</t>
+  </si>
+  <si>
+    <t>Day1\After Drug\HighFreq_6</t>
+  </si>
+  <si>
+    <t>Day1\After Drug\HighFreq_7</t>
+  </si>
+  <si>
+    <t>Day1\After Drug\HighFreq_8</t>
+  </si>
+  <si>
+    <t>Day1\After Drug\HighFreq_9</t>
+  </si>
+  <si>
+    <t>Day1\After Drug\HighFreq_10</t>
+  </si>
+  <si>
+    <t>Day1\After Drug\HighFreq_11</t>
+  </si>
+  <si>
+    <t>Day1\After Drug\HighFreq_12</t>
+  </si>
+  <si>
+    <t>Day1\After Drug\HighFreq_13</t>
+  </si>
+  <si>
+    <t>Day1\After Drug\HighFreq_14</t>
+  </si>
+  <si>
+    <t>Day1\After Drug\HighFreq_15</t>
+  </si>
+  <si>
+    <t>Day1\After Drug\HighFreq_16</t>
+  </si>
+  <si>
+    <t>Day1\After Drug\HighFreq_17</t>
+  </si>
+  <si>
+    <t>Day1\After Drug\HighFreq_18</t>
+  </si>
+  <si>
+    <t>Day1\After Drug\HighFreq_19</t>
+  </si>
+  <si>
+    <t>Day1\After Drug\HighFreq_20</t>
+  </si>
+  <si>
+    <t>Day1\After Drug\HighFreq_21</t>
+  </si>
+  <si>
+    <t>Day1\After Drug\HighFreq_22</t>
+  </si>
+  <si>
+    <t>Day1\After Drug\HighFreq_23</t>
+  </si>
+  <si>
+    <t>Day1\After Drug\HighFreq_24</t>
+  </si>
+  <si>
+    <t>Day1\After Drug\HighFreq_25</t>
+  </si>
+  <si>
+    <t>Day1\After Drug\HighFreq_26</t>
+  </si>
+  <si>
+    <t>Day1\After Drug\HighFreq_27</t>
+  </si>
+  <si>
+    <t>Day1\After Drug\HighFreq_28</t>
+  </si>
+  <si>
+    <t>Day1\After Drug\HighFreq_29</t>
+  </si>
+  <si>
+    <t>Day1\After Drug\HighFreq_30</t>
+  </si>
+  <si>
+    <t>Day1\After Drug\HighFreq_31</t>
+  </si>
+  <si>
+    <t>Day1\After Drug\HighFreq_32</t>
+  </si>
+  <si>
+    <t>Day1\After Drug\HighFreq_33</t>
+  </si>
+  <si>
+    <t>Day1\After Drug\HighFreq_34</t>
+  </si>
+  <si>
+    <t>Day1\After Drug\HighFreq_35</t>
+  </si>
+  <si>
+    <t>Day1\After Drug\HighFreq_36</t>
+  </si>
+  <si>
+    <t>Day1\After Drug\HighFreq_37</t>
+  </si>
+  <si>
+    <t>Day1\After Drug\HighFreq_38</t>
+  </si>
+  <si>
+    <t>Day1\After Drug\HighFreq_39</t>
+  </si>
+  <si>
+    <t>Day1\After Drug\HighFreq_40</t>
+  </si>
+  <si>
+    <t>Day1\After Drug\HighFreq_41</t>
+  </si>
+  <si>
+    <t>Day1\After Drug\HighFreq_42</t>
+  </si>
+  <si>
+    <t>Day1\After Drug\HighFreq_43</t>
+  </si>
+  <si>
+    <t>Day1\After Drug\HighFreq_44</t>
+  </si>
+  <si>
+    <t>Day1\After Drug\HighFreq_45</t>
+  </si>
+  <si>
+    <t>Day1\After Drug\HighFreq_46</t>
+  </si>
+  <si>
+    <t>Day1\After Drug\HighFreq_47</t>
+  </si>
+  <si>
+    <t>Day1\After Drug\HighFreq_48</t>
+  </si>
+  <si>
+    <t>Day1\After Drug\HighFreq_49</t>
+  </si>
+  <si>
+    <t>Day2\HighFreq_1</t>
+  </si>
+  <si>
+    <t>Day2\HighFreq_2</t>
+  </si>
+  <si>
+    <t>Day2\HighFreq_3</t>
+  </si>
+  <si>
+    <t>Day2\HighFreq_4</t>
+  </si>
+  <si>
+    <t>Day2\HighFreq_5</t>
+  </si>
+  <si>
+    <t>Day2\HighFreq_6</t>
+  </si>
+  <si>
+    <t>Day2\HighFreq_7</t>
+  </si>
+  <si>
+    <t>Day2\HighFreq_8</t>
+  </si>
+  <si>
+    <t>Day2\HighFreq_9</t>
+  </si>
+  <si>
+    <t>Day2\HighFreq_10</t>
+  </si>
+  <si>
+    <t>Day2\HighFreq_11</t>
+  </si>
+  <si>
+    <t>Day2\HighFreq_12</t>
+  </si>
+  <si>
+    <t>Day2\HighFreq_13</t>
+  </si>
+  <si>
+    <t>Day2\HighFreq_14</t>
+  </si>
+  <si>
+    <t>Day2\HighFreq_15</t>
+  </si>
+  <si>
+    <t>Day2\HighFreq_16</t>
+  </si>
+  <si>
+    <t>Day2\HighFreq_17</t>
+  </si>
+  <si>
+    <t>Day2\HighFreq_18</t>
+  </si>
+  <si>
+    <t>Day2\HighFreq_19</t>
+  </si>
+  <si>
+    <t>ZB</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_1</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_2</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_3</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_4</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_5</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_6</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_7</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_8</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_9</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_10</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_11</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_12</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_13</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_14</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_15</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_16</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_17</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_18</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_19</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_20</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_21</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_22</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_23</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_24</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_25</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_26</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_27</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_28</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_29</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_30</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_31</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_32</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_33</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_34</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_35</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_36</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_37</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_38</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_39</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_40</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_41</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_42</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_43</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_44</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_45</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_46</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_47</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_48</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_49</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_50</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_51</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_52</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_53</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_54</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_55</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_56</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_57</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_58</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_59</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_60</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_61</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_62</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_63</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_64</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_65</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_66</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_67</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_68</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_69</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_70</t>
+  </si>
+  <si>
+    <t>Day3\HighFreq_71</t>
   </si>
 </sst>
 </file>
@@ -669,12 +939,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J83"/>
+  <dimension ref="A1:J183"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A149" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="L63" sqref="L63"/>
+      <selection pane="bottomLeft" activeCell="F162" sqref="F162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -696,10 +966,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>73</v>
+        <v>6</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>74</v>
+        <v>7</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>1</v>
@@ -717,19 +987,19 @@
         <v>5</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>76</v>
+        <v>8</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>77</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D2" s="6">
         <v>1</v>
@@ -755,11 +1025,11 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D3" s="6">
         <v>1</v>
@@ -785,11 +1055,11 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D4" s="6">
         <v>1</v>
@@ -815,11 +1085,11 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D5" s="6">
         <v>1</v>
@@ -845,11 +1115,11 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D6" s="6">
         <v>1</v>
@@ -875,11 +1145,11 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D7" s="6">
         <v>1</v>
@@ -905,11 +1175,11 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D8" s="6">
         <v>1</v>
@@ -935,11 +1205,11 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D9" s="6">
         <v>1</v>
@@ -965,11 +1235,11 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D10" s="6">
         <v>1</v>
@@ -995,11 +1265,11 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D11" s="6">
         <v>1</v>
@@ -1025,11 +1295,11 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D12" s="6">
         <v>1</v>
@@ -1055,11 +1325,11 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D13" s="6">
         <v>1</v>
@@ -1085,11 +1355,11 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D14" s="6">
         <v>1</v>
@@ -1115,11 +1385,11 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D15" s="6">
         <v>1</v>
@@ -1145,11 +1415,11 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D16" s="6">
         <v>1</v>
@@ -1175,11 +1445,11 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D17" s="6">
         <v>1</v>
@@ -1205,11 +1475,11 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D18" s="6">
         <v>1</v>
@@ -1235,11 +1505,11 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D19" s="6">
         <v>1</v>
@@ -1265,13 +1535,13 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B20" s="7">
         <v>42857.972222222219</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D20" s="6">
         <v>1</v>
@@ -1297,13 +1567,13 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B21" s="7">
         <v>42857.972222222219</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D21" s="6">
         <v>1</v>
@@ -1329,13 +1599,13 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B22" s="7">
         <v>42857.972222222219</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D22" s="6">
         <v>1</v>
@@ -1361,13 +1631,13 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B23" s="7">
         <v>42857.972222222219</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D23" s="6">
         <v>1</v>
@@ -1393,13 +1663,13 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B24" s="7">
         <v>42857.972222222219</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D24" s="6">
         <v>1</v>
@@ -1425,13 +1695,13 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B25" s="7">
         <v>42857.972222222219</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D25" s="6">
         <v>1</v>
@@ -1457,13 +1727,13 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B26" s="7">
         <v>42857.972222222219</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D26" s="6">
         <v>1</v>
@@ -1489,13 +1759,13 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B27" s="7">
         <v>42857.972222222219</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D27" s="6">
         <v>1</v>
@@ -1521,13 +1791,13 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B28" s="7">
         <v>42857.972222222219</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D28" s="6">
         <v>1</v>
@@ -1553,13 +1823,13 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B29" s="7">
         <v>42857.972222222219</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D29" s="6">
         <v>1</v>
@@ -1585,13 +1855,13 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B30" s="7">
         <v>42857.972222222219</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D30" s="6">
         <v>1</v>
@@ -1617,13 +1887,13 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B31" s="7">
         <v>42857.972222222219</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D31" s="6">
         <v>1</v>
@@ -1649,13 +1919,13 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B32" s="7">
         <v>42857.972222222219</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D32" s="6">
         <v>1</v>
@@ -1681,13 +1951,13 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B33" s="7">
         <v>42857.972222222219</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D33" s="6">
         <v>1</v>
@@ -1713,13 +1983,13 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B34" s="7">
         <v>42857.972222222219</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D34" s="6">
         <v>1</v>
@@ -1745,13 +2015,13 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B35" s="7">
         <v>42857.972222222219</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D35" s="6">
         <v>1</v>
@@ -1777,13 +2047,13 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B36" s="7">
         <v>42857.972222222219</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D36" s="6">
         <v>1</v>
@@ -1809,13 +2079,13 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B37" s="7">
         <v>42857.972222222219</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D37" s="6">
         <v>1</v>
@@ -1841,13 +2111,13 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B38" s="7">
         <v>42857.972222222219</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D38" s="6">
         <v>1</v>
@@ -1873,13 +2143,13 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B39" s="7">
         <v>42857.972222222219</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D39" s="6">
         <v>1</v>
@@ -1905,13 +2175,13 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B40" s="7">
         <v>42857.972222222219</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D40" s="6">
         <v>1</v>
@@ -1937,13 +2207,13 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B41" s="7">
         <v>42857.972222222219</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D41" s="6">
         <v>1</v>
@@ -1969,13 +2239,13 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B42" s="7">
         <v>42857.972222222219</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D42" s="6">
         <v>1</v>
@@ -2001,13 +2271,13 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B43" s="7">
         <v>42857.972222222219</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D43" s="6">
         <v>1</v>
@@ -2033,13 +2303,13 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B44" s="7">
         <v>42857.972222222219</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D44" s="6">
         <v>1</v>
@@ -2065,13 +2335,13 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B45" s="7">
         <v>42857.972222222219</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D45" s="6">
         <v>1</v>
@@ -2097,13 +2367,13 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B46" s="7">
         <v>42857.972222222219</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D46" s="6">
         <v>1</v>
@@ -2129,13 +2399,13 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B47" s="7">
         <v>42857.972222222219</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D47" s="6">
         <v>1</v>
@@ -2161,13 +2431,13 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B48" s="7">
         <v>42857.972222222219</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D48" s="6">
         <v>1</v>
@@ -2193,13 +2463,13 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B49" s="7">
         <v>42857.972222222219</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D49" s="6">
         <v>1</v>
@@ -2225,13 +2495,13 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B50" s="7">
         <v>42857.972222222219</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D50" s="6">
         <v>1</v>
@@ -2257,13 +2527,13 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B51" s="7">
         <v>42857.972222222219</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D51" s="6">
         <v>1</v>
@@ -2289,13 +2559,13 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B52" s="7">
         <v>42857.972222222219</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D52" s="6">
         <v>1</v>
@@ -2321,13 +2591,13 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B53" s="7">
         <v>42857.972222222219</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D53" s="6">
         <v>1</v>
@@ -2353,13 +2623,13 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B54" s="7">
         <v>42857.972222222219</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D54" s="6">
         <v>1</v>
@@ -2385,13 +2655,13 @@
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B55" s="7">
         <v>42857.972222222219</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D55" s="6">
         <v>1</v>
@@ -2417,13 +2687,13 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B56" s="7">
         <v>42857.972222222219</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D56" s="6">
         <v>1</v>
@@ -2449,13 +2719,13 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B57" s="7">
         <v>42857.972222222219</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D57" s="6">
         <v>1</v>
@@ -2481,13 +2751,13 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B58" s="7">
         <v>42857.972222222219</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D58" s="6">
         <v>1</v>
@@ -2513,13 +2783,13 @@
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B59" s="7">
         <v>42857.972222222219</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D59" s="6">
         <v>1</v>
@@ -2545,13 +2815,13 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B60" s="7">
         <v>42857.972222222219</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D60" s="6">
         <v>1</v>
@@ -2577,13 +2847,13 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B61" s="7">
         <v>42857.972222222219</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D61" s="6">
         <v>1</v>
@@ -2609,13 +2879,13 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B62" s="7">
         <v>42857.972222222219</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D62" s="6">
         <v>1</v>
@@ -2641,13 +2911,13 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B63" s="7">
         <v>42857.972222222219</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D63" s="6">
         <v>1</v>
@@ -2673,13 +2943,13 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B64" s="7">
         <v>42857.972222222219</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D64" s="6">
         <v>1</v>
@@ -2705,13 +2975,13 @@
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B65" s="7">
         <v>42857.972222222219</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D65" s="6">
         <v>1</v>
@@ -2737,13 +3007,13 @@
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B66" s="7">
         <v>42857.972222222219</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D66" s="6">
         <v>1</v>
@@ -2769,13 +3039,13 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B67" s="7">
         <v>42857.972222222219</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D67" s="6">
         <v>1</v>
@@ -2801,13 +3071,13 @@
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B68" s="7">
         <v>42857.972222222219</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D68" s="6">
         <v>1</v>
@@ -2832,64 +3102,3059 @@
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E69" s="6"/>
-      <c r="F69" s="6"/>
+      <c r="A69" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B69" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D69" s="6">
+        <v>1</v>
+      </c>
+      <c r="E69" s="6">
+        <v>3</v>
+      </c>
+      <c r="F69" s="6">
+        <v>3</v>
+      </c>
+      <c r="G69" s="6">
+        <v>19</v>
+      </c>
+      <c r="H69" s="6">
+        <v>1</v>
+      </c>
+      <c r="I69" s="8">
+        <v>42859.359027777777</v>
+      </c>
+      <c r="J69">
+        <v>1.3868055555576575</v>
+      </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E70" s="6"/>
-      <c r="F70" s="6"/>
+      <c r="A70" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B70" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D70" s="6">
+        <v>1</v>
+      </c>
+      <c r="E70" s="6">
+        <v>3</v>
+      </c>
+      <c r="F70" s="6">
+        <v>4</v>
+      </c>
+      <c r="G70" s="6">
+        <v>20</v>
+      </c>
+      <c r="H70" s="6">
+        <v>1</v>
+      </c>
+      <c r="I70" s="8">
+        <v>42859.369444444441</v>
+      </c>
+      <c r="J70">
+        <v>1.3972222222218988</v>
+      </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E71" s="6"/>
-      <c r="F71" s="6"/>
+      <c r="A71" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B71" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C71" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D71" s="6">
+        <v>1</v>
+      </c>
+      <c r="E71" s="6">
+        <v>3</v>
+      </c>
+      <c r="F71" s="6">
+        <v>5</v>
+      </c>
+      <c r="G71" s="6">
+        <v>21</v>
+      </c>
+      <c r="H71" s="6">
+        <v>1</v>
+      </c>
+      <c r="I71" s="8">
+        <v>42859.379861111105</v>
+      </c>
+      <c r="J71">
+        <v>1.4076388888861402</v>
+      </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E72" s="6"/>
-      <c r="F72" s="6"/>
+      <c r="A72" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B72" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C72" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D72" s="6">
+        <v>1</v>
+      </c>
+      <c r="E72" s="6">
+        <v>3</v>
+      </c>
+      <c r="F72" s="6">
+        <v>6</v>
+      </c>
+      <c r="G72" s="6">
+        <v>22</v>
+      </c>
+      <c r="H72" s="6">
+        <v>1</v>
+      </c>
+      <c r="I72" s="8">
+        <v>42859.390277777769</v>
+      </c>
+      <c r="J72">
+        <v>1.4180555555503815</v>
+      </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E73" s="6"/>
-      <c r="F73" s="6"/>
+      <c r="A73" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B73" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C73" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D73" s="6">
+        <v>1</v>
+      </c>
+      <c r="E73" s="6">
+        <v>3</v>
+      </c>
+      <c r="F73" s="6">
+        <v>7</v>
+      </c>
+      <c r="G73" s="6">
+        <v>23</v>
+      </c>
+      <c r="H73" s="6">
+        <v>1</v>
+      </c>
+      <c r="I73" s="8">
+        <v>42859.400694444434</v>
+      </c>
+      <c r="J73">
+        <v>1.4284722222146229</v>
+      </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E74" s="6"/>
-      <c r="F74" s="6"/>
+      <c r="A74" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B74" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C74" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D74" s="6">
+        <v>1</v>
+      </c>
+      <c r="E74" s="6">
+        <v>3</v>
+      </c>
+      <c r="F74" s="6">
+        <v>8</v>
+      </c>
+      <c r="G74" s="6">
+        <v>24</v>
+      </c>
+      <c r="H74" s="6">
+        <v>1</v>
+      </c>
+      <c r="I74" s="8">
+        <v>42859.411111111098</v>
+      </c>
+      <c r="J74">
+        <v>1.4388888888788642</v>
+      </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E75" s="6"/>
-      <c r="F75" s="6"/>
+      <c r="A75" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B75" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C75" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D75" s="6">
+        <v>1</v>
+      </c>
+      <c r="E75" s="6">
+        <v>3</v>
+      </c>
+      <c r="F75" s="6">
+        <v>9</v>
+      </c>
+      <c r="G75" s="6">
+        <v>25</v>
+      </c>
+      <c r="H75" s="6">
+        <v>1</v>
+      </c>
+      <c r="I75" s="8">
+        <v>42859.421527777762</v>
+      </c>
+      <c r="J75">
+        <v>1.4493055555431056</v>
+      </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E76" s="6"/>
-      <c r="F76" s="6"/>
+      <c r="A76" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B76" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D76" s="6">
+        <v>1</v>
+      </c>
+      <c r="E76" s="6">
+        <v>3</v>
+      </c>
+      <c r="F76" s="6">
+        <v>10</v>
+      </c>
+      <c r="G76" s="6">
+        <v>26</v>
+      </c>
+      <c r="H76" s="6">
+        <v>1</v>
+      </c>
+      <c r="I76" s="8">
+        <v>42859.431944444426</v>
+      </c>
+      <c r="J76">
+        <v>1.4597222222073469</v>
+      </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E77" s="6"/>
-      <c r="F77" s="6"/>
+      <c r="A77" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B77" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C77" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D77" s="6">
+        <v>1</v>
+      </c>
+      <c r="E77" s="6">
+        <v>4</v>
+      </c>
+      <c r="F77" s="6">
+        <v>3</v>
+      </c>
+      <c r="G77" s="6">
+        <v>27</v>
+      </c>
+      <c r="H77" s="6">
+        <v>1</v>
+      </c>
+      <c r="I77" s="8">
+        <v>42859.442361111091</v>
+      </c>
+      <c r="J77">
+        <v>1.4701388888715883</v>
+      </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E78" s="6"/>
-      <c r="F78" s="6"/>
+      <c r="A78" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B78" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C78" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D78" s="6">
+        <v>1</v>
+      </c>
+      <c r="E78" s="6">
+        <v>4</v>
+      </c>
+      <c r="F78" s="6">
+        <v>4</v>
+      </c>
+      <c r="G78" s="6">
+        <v>28</v>
+      </c>
+      <c r="H78" s="6">
+        <v>1</v>
+      </c>
+      <c r="I78" s="8">
+        <v>42859.452777777755</v>
+      </c>
+      <c r="J78">
+        <v>1.4805555555358296</v>
+      </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E79" s="6"/>
-      <c r="F79" s="6"/>
+      <c r="A79" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B79" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C79" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D79" s="6">
+        <v>1</v>
+      </c>
+      <c r="E79" s="6">
+        <v>4</v>
+      </c>
+      <c r="F79" s="6">
+        <v>5</v>
+      </c>
+      <c r="G79" s="6">
+        <v>29</v>
+      </c>
+      <c r="H79" s="6">
+        <v>1</v>
+      </c>
+      <c r="I79" s="8">
+        <v>42859.463194444419</v>
+      </c>
+      <c r="J79">
+        <v>1.490972222200071</v>
+      </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E80" s="6"/>
-      <c r="F80" s="6"/>
-    </row>
-    <row r="81" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E81" s="6"/>
-      <c r="F81" s="6"/>
-    </row>
-    <row r="82" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E82" s="6"/>
-      <c r="F82" s="6"/>
-    </row>
-    <row r="83" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E83" s="6"/>
-      <c r="F83" s="6"/>
+      <c r="A80" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B80" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C80" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D80" s="6">
+        <v>1</v>
+      </c>
+      <c r="E80" s="6">
+        <v>4</v>
+      </c>
+      <c r="F80" s="6">
+        <v>6</v>
+      </c>
+      <c r="G80" s="6">
+        <v>30</v>
+      </c>
+      <c r="H80" s="6">
+        <v>1</v>
+      </c>
+      <c r="I80" s="8">
+        <v>42859.473611111083</v>
+      </c>
+      <c r="J80">
+        <v>1.5013888888643123</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B81" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C81" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D81" s="6">
+        <v>1</v>
+      </c>
+      <c r="E81" s="6">
+        <v>4</v>
+      </c>
+      <c r="F81" s="6">
+        <v>7</v>
+      </c>
+      <c r="G81" s="6">
+        <v>31</v>
+      </c>
+      <c r="H81" s="6">
+        <v>1</v>
+      </c>
+      <c r="I81" s="8">
+        <v>42859.484027777748</v>
+      </c>
+      <c r="J81">
+        <v>1.5118055555285537</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B82" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C82" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D82" s="6">
+        <v>1</v>
+      </c>
+      <c r="E82" s="6">
+        <v>4</v>
+      </c>
+      <c r="F82" s="6">
+        <v>8</v>
+      </c>
+      <c r="G82" s="6">
+        <v>32</v>
+      </c>
+      <c r="H82" s="6">
+        <v>1</v>
+      </c>
+      <c r="I82" s="8">
+        <v>42859.494444444412</v>
+      </c>
+      <c r="J82">
+        <v>1.522222222192795</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B83" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C83" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D83" s="6">
+        <v>1</v>
+      </c>
+      <c r="E83" s="6">
+        <v>4</v>
+      </c>
+      <c r="F83" s="6">
+        <v>9</v>
+      </c>
+      <c r="G83" s="6">
+        <v>33</v>
+      </c>
+      <c r="H83" s="6">
+        <v>1</v>
+      </c>
+      <c r="I83" s="8">
+        <v>42859.504861111076</v>
+      </c>
+      <c r="J83">
+        <v>1.5326388888570364</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B84" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C84" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D84" s="6">
+        <v>1</v>
+      </c>
+      <c r="E84" s="6">
+        <v>4</v>
+      </c>
+      <c r="F84" s="6">
+        <v>10</v>
+      </c>
+      <c r="G84" s="6">
+        <v>34</v>
+      </c>
+      <c r="H84" s="6">
+        <v>1</v>
+      </c>
+      <c r="I84" s="8">
+        <v>42859.51527777774</v>
+      </c>
+      <c r="J84">
+        <v>1.5430555555212777</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B85" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C85" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D85" s="6">
+        <v>1</v>
+      </c>
+      <c r="E85" s="6">
+        <v>5</v>
+      </c>
+      <c r="F85" s="6">
+        <v>3</v>
+      </c>
+      <c r="G85" s="6">
+        <v>35</v>
+      </c>
+      <c r="H85" s="6">
+        <v>1</v>
+      </c>
+      <c r="I85" s="8">
+        <v>42859.525694444405</v>
+      </c>
+      <c r="J85">
+        <v>1.5534722221855191</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B86" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C86" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D86" s="6">
+        <v>1</v>
+      </c>
+      <c r="E86" s="6">
+        <v>5</v>
+      </c>
+      <c r="F86" s="6">
+        <v>4</v>
+      </c>
+      <c r="G86" s="6">
+        <v>36</v>
+      </c>
+      <c r="H86" s="6">
+        <v>1</v>
+      </c>
+      <c r="I86" s="8">
+        <v>42859.536111111069</v>
+      </c>
+      <c r="J86">
+        <v>1.5638888888497604</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B87" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C87" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D87" s="6">
+        <v>1</v>
+      </c>
+      <c r="E87" s="6">
+        <v>5</v>
+      </c>
+      <c r="F87" s="6">
+        <v>5</v>
+      </c>
+      <c r="G87" s="6">
+        <v>37</v>
+      </c>
+      <c r="H87" s="6">
+        <v>1</v>
+      </c>
+      <c r="I87" s="8">
+        <v>42859.546527777733</v>
+      </c>
+      <c r="J87">
+        <v>1.5743055555140018</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B88" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C88" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D88" s="6">
+        <v>1</v>
+      </c>
+      <c r="E88" s="6">
+        <v>3</v>
+      </c>
+      <c r="F88" s="6">
+        <v>3</v>
+      </c>
+      <c r="G88" s="6">
+        <v>1</v>
+      </c>
+      <c r="H88" s="6">
+        <v>1</v>
+      </c>
+      <c r="I88" s="8">
+        <v>42859.3125</v>
+      </c>
+      <c r="J88">
+        <v>1.3402777777810115</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B89" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C89" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D89" s="6">
+        <v>1</v>
+      </c>
+      <c r="E89" s="6">
+        <v>3</v>
+      </c>
+      <c r="F89" s="6">
+        <v>4</v>
+      </c>
+      <c r="G89" s="6">
+        <v>2</v>
+      </c>
+      <c r="H89" s="6">
+        <v>1</v>
+      </c>
+      <c r="I89" s="8">
+        <v>42859.322916666664</v>
+      </c>
+      <c r="J89">
+        <v>1.3506944444452529</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B90" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C90" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D90" s="6">
+        <v>1</v>
+      </c>
+      <c r="E90" s="6">
+        <v>3</v>
+      </c>
+      <c r="F90" s="6">
+        <v>5</v>
+      </c>
+      <c r="G90" s="6">
+        <v>3</v>
+      </c>
+      <c r="H90" s="6">
+        <v>1</v>
+      </c>
+      <c r="I90" s="8">
+        <v>42859.333333333328</v>
+      </c>
+      <c r="J90">
+        <v>1.3611111111094942</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B91" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C91" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D91" s="6">
+        <v>1</v>
+      </c>
+      <c r="E91" s="6">
+        <v>3</v>
+      </c>
+      <c r="F91" s="6">
+        <v>6</v>
+      </c>
+      <c r="G91" s="6">
+        <v>4</v>
+      </c>
+      <c r="H91" s="6">
+        <v>1</v>
+      </c>
+      <c r="I91" s="8">
+        <v>42859.343749999993</v>
+      </c>
+      <c r="J91">
+        <v>1.3715277777737356</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B92" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C92" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D92" s="6">
+        <v>1</v>
+      </c>
+      <c r="E92" s="6">
+        <v>3</v>
+      </c>
+      <c r="F92" s="6">
+        <v>7</v>
+      </c>
+      <c r="G92" s="6">
+        <v>5</v>
+      </c>
+      <c r="H92" s="6">
+        <v>1</v>
+      </c>
+      <c r="I92" s="8">
+        <v>42859.354166666657</v>
+      </c>
+      <c r="J92">
+        <v>1.3819444444379769</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B93" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C93" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D93" s="6">
+        <v>1</v>
+      </c>
+      <c r="E93" s="6">
+        <v>3</v>
+      </c>
+      <c r="F93" s="6">
+        <v>8</v>
+      </c>
+      <c r="G93" s="6">
+        <v>6</v>
+      </c>
+      <c r="H93" s="6">
+        <v>1</v>
+      </c>
+      <c r="I93" s="8">
+        <v>42859.364583333321</v>
+      </c>
+      <c r="J93">
+        <v>1.3923611111022183</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B94" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C94" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D94" s="6">
+        <v>1</v>
+      </c>
+      <c r="E94" s="6">
+        <v>3</v>
+      </c>
+      <c r="F94" s="6">
+        <v>9</v>
+      </c>
+      <c r="G94" s="6">
+        <v>7</v>
+      </c>
+      <c r="H94" s="6">
+        <v>1</v>
+      </c>
+      <c r="I94" s="8">
+        <v>42859.374999999985</v>
+      </c>
+      <c r="J94">
+        <v>1.4027777777664596</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B95" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C95" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D95" s="6">
+        <v>1</v>
+      </c>
+      <c r="E95" s="6">
+        <v>3</v>
+      </c>
+      <c r="F95" s="6">
+        <v>10</v>
+      </c>
+      <c r="G95" s="6">
+        <v>8</v>
+      </c>
+      <c r="H95" s="6">
+        <v>1</v>
+      </c>
+      <c r="I95" s="8">
+        <v>42859.38541666665</v>
+      </c>
+      <c r="J95">
+        <v>1.413194444430701</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B96" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C96" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D96" s="6">
+        <v>1</v>
+      </c>
+      <c r="E96" s="6">
+        <v>4</v>
+      </c>
+      <c r="F96" s="6">
+        <v>3</v>
+      </c>
+      <c r="G96" s="6">
+        <v>9</v>
+      </c>
+      <c r="H96" s="6">
+        <v>1</v>
+      </c>
+      <c r="I96" s="8">
+        <v>42859.395833333314</v>
+      </c>
+      <c r="J96">
+        <v>1.4236111110949423</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B97" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C97" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D97" s="6">
+        <v>1</v>
+      </c>
+      <c r="E97" s="6">
+        <v>4</v>
+      </c>
+      <c r="F97" s="6">
+        <v>4</v>
+      </c>
+      <c r="G97" s="6">
+        <v>10</v>
+      </c>
+      <c r="H97" s="6">
+        <v>1</v>
+      </c>
+      <c r="I97" s="8">
+        <v>42859.406249999978</v>
+      </c>
+      <c r="J97">
+        <v>1.4340277777591837</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B98" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C98" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D98" s="6">
+        <v>1</v>
+      </c>
+      <c r="E98" s="6">
+        <v>4</v>
+      </c>
+      <c r="F98" s="6">
+        <v>5</v>
+      </c>
+      <c r="G98" s="6">
+        <v>11</v>
+      </c>
+      <c r="H98" s="6">
+        <v>1</v>
+      </c>
+      <c r="I98" s="8">
+        <v>42859.416666666642</v>
+      </c>
+      <c r="J98">
+        <v>1.444444444423425</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B99" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C99" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D99" s="6">
+        <v>1</v>
+      </c>
+      <c r="E99" s="6">
+        <v>4</v>
+      </c>
+      <c r="F99" s="6">
+        <v>6</v>
+      </c>
+      <c r="G99" s="6">
+        <v>12</v>
+      </c>
+      <c r="H99" s="6">
+        <v>1</v>
+      </c>
+      <c r="I99" s="8">
+        <v>42859.427083333307</v>
+      </c>
+      <c r="J99">
+        <v>1.4548611110876664</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B100" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C100" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D100" s="6">
+        <v>1</v>
+      </c>
+      <c r="E100" s="6">
+        <v>4</v>
+      </c>
+      <c r="F100" s="6">
+        <v>7</v>
+      </c>
+      <c r="G100" s="6">
+        <v>13</v>
+      </c>
+      <c r="H100" s="6">
+        <v>1</v>
+      </c>
+      <c r="I100" s="8">
+        <v>42859.437499999971</v>
+      </c>
+      <c r="J100">
+        <v>1.4652777777519077</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B101" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C101" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D101" s="6">
+        <v>1</v>
+      </c>
+      <c r="E101" s="6">
+        <v>4</v>
+      </c>
+      <c r="F101" s="6">
+        <v>8</v>
+      </c>
+      <c r="G101" s="6">
+        <v>14</v>
+      </c>
+      <c r="H101" s="6">
+        <v>1</v>
+      </c>
+      <c r="I101" s="8">
+        <v>42859.447916666635</v>
+      </c>
+      <c r="J101">
+        <v>1.4756944444161491</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B102" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C102" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D102" s="6">
+        <v>1</v>
+      </c>
+      <c r="E102" s="6">
+        <v>4</v>
+      </c>
+      <c r="F102" s="6">
+        <v>9</v>
+      </c>
+      <c r="G102" s="6">
+        <v>15</v>
+      </c>
+      <c r="H102" s="6">
+        <v>1</v>
+      </c>
+      <c r="I102" s="8">
+        <v>42859.458333333299</v>
+      </c>
+      <c r="J102">
+        <v>1.4861111110803904</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A103" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B103" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C103" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D103" s="6">
+        <v>1</v>
+      </c>
+      <c r="E103" s="6">
+        <v>4</v>
+      </c>
+      <c r="F103" s="6">
+        <v>10</v>
+      </c>
+      <c r="G103" s="6">
+        <v>16</v>
+      </c>
+      <c r="H103" s="6">
+        <v>1</v>
+      </c>
+      <c r="I103" s="8">
+        <v>42859.468749999964</v>
+      </c>
+      <c r="J103">
+        <v>1.4965277777446317</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A104" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B104" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C104" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D104" s="6">
+        <v>1</v>
+      </c>
+      <c r="E104" s="6">
+        <v>5</v>
+      </c>
+      <c r="F104" s="6">
+        <v>3</v>
+      </c>
+      <c r="G104" s="6">
+        <v>17</v>
+      </c>
+      <c r="H104" s="6">
+        <v>1</v>
+      </c>
+      <c r="I104" s="8">
+        <v>42859.479166666628</v>
+      </c>
+      <c r="J104">
+        <v>1.5069444444088731</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A105" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B105" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C105" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D105" s="6">
+        <v>1</v>
+      </c>
+      <c r="E105" s="6">
+        <v>5</v>
+      </c>
+      <c r="F105" s="6">
+        <v>4</v>
+      </c>
+      <c r="G105" s="6">
+        <v>18</v>
+      </c>
+      <c r="H105" s="6">
+        <v>1</v>
+      </c>
+      <c r="I105" s="8">
+        <v>42859.489583333292</v>
+      </c>
+      <c r="J105">
+        <v>1.5173611110731144</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A106" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B106" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C106" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D106" s="6">
+        <v>1</v>
+      </c>
+      <c r="E106" s="6">
+        <v>3</v>
+      </c>
+      <c r="F106" s="6">
+        <v>3</v>
+      </c>
+      <c r="G106" s="6">
+        <v>19</v>
+      </c>
+      <c r="H106" s="6">
+        <v>1</v>
+      </c>
+      <c r="I106" s="8">
+        <v>42859.499999999956</v>
+      </c>
+      <c r="J106">
+        <v>1.5277777777373558</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A107" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B107" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C107" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D107" s="6">
+        <v>1</v>
+      </c>
+      <c r="E107" s="6">
+        <v>3</v>
+      </c>
+      <c r="F107" s="6">
+        <v>4</v>
+      </c>
+      <c r="G107" s="6">
+        <v>20</v>
+      </c>
+      <c r="H107" s="6">
+        <v>1</v>
+      </c>
+      <c r="I107" s="8">
+        <v>42859.510416666621</v>
+      </c>
+      <c r="J107">
+        <v>1.5381944444015971</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A108" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B108" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C108" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D108" s="6">
+        <v>1</v>
+      </c>
+      <c r="E108" s="6">
+        <v>3</v>
+      </c>
+      <c r="F108" s="6">
+        <v>5</v>
+      </c>
+      <c r="G108" s="6">
+        <v>21</v>
+      </c>
+      <c r="H108" s="6">
+        <v>1</v>
+      </c>
+      <c r="I108" s="8">
+        <v>42859.520833333285</v>
+      </c>
+      <c r="J108">
+        <v>1.5486111110658385</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A109" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B109" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C109" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D109" s="6">
+        <v>1</v>
+      </c>
+      <c r="E109" s="6">
+        <v>3</v>
+      </c>
+      <c r="F109" s="6">
+        <v>6</v>
+      </c>
+      <c r="G109" s="6">
+        <v>22</v>
+      </c>
+      <c r="H109" s="6">
+        <v>1</v>
+      </c>
+      <c r="I109" s="8">
+        <v>42859.531249999949</v>
+      </c>
+      <c r="J109">
+        <v>1.5590277777300798</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A110" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B110" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C110" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D110" s="6">
+        <v>1</v>
+      </c>
+      <c r="E110" s="6">
+        <v>3</v>
+      </c>
+      <c r="F110" s="6">
+        <v>7</v>
+      </c>
+      <c r="G110" s="6">
+        <v>23</v>
+      </c>
+      <c r="H110" s="6">
+        <v>1</v>
+      </c>
+      <c r="I110" s="8">
+        <v>42859.541666666613</v>
+      </c>
+      <c r="J110">
+        <v>1.5694444443943212</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A111" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B111" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C111" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D111" s="6">
+        <v>1</v>
+      </c>
+      <c r="E111" s="6">
+        <v>3</v>
+      </c>
+      <c r="F111" s="6">
+        <v>8</v>
+      </c>
+      <c r="G111" s="6">
+        <v>24</v>
+      </c>
+      <c r="H111" s="6">
+        <v>1</v>
+      </c>
+      <c r="I111" s="8">
+        <v>42859.552083333278</v>
+      </c>
+      <c r="J111">
+        <v>1.5798611110585625</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A112" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B112" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C112" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D112" s="6">
+        <v>1</v>
+      </c>
+      <c r="E112" s="6">
+        <v>3</v>
+      </c>
+      <c r="F112" s="6">
+        <v>9</v>
+      </c>
+      <c r="G112" s="6">
+        <v>25</v>
+      </c>
+      <c r="H112" s="6">
+        <v>1</v>
+      </c>
+      <c r="I112" s="8">
+        <v>42859.562499999942</v>
+      </c>
+      <c r="J112">
+        <v>1.5902777777228039</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A113" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B113" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C113" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D113" s="6">
+        <v>1</v>
+      </c>
+      <c r="E113" s="6">
+        <v>3</v>
+      </c>
+      <c r="F113" s="6">
+        <v>10</v>
+      </c>
+      <c r="G113" s="6">
+        <v>26</v>
+      </c>
+      <c r="H113" s="6">
+        <v>1</v>
+      </c>
+      <c r="I113" s="8">
+        <v>42859.572916666606</v>
+      </c>
+      <c r="J113">
+        <v>1.6006944443870452</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A114" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B114" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C114" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D114" s="6">
+        <v>1</v>
+      </c>
+      <c r="E114" s="6">
+        <v>4</v>
+      </c>
+      <c r="F114" s="6">
+        <v>3</v>
+      </c>
+      <c r="G114" s="6">
+        <v>27</v>
+      </c>
+      <c r="H114" s="6">
+        <v>1</v>
+      </c>
+      <c r="I114" s="8">
+        <v>42859.58333333327</v>
+      </c>
+      <c r="J114">
+        <v>1.6111111110512866</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A115" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="B115" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C115" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D115" s="6">
+        <v>1</v>
+      </c>
+      <c r="E115" s="6">
+        <v>4</v>
+      </c>
+      <c r="F115" s="6">
+        <v>4</v>
+      </c>
+      <c r="G115" s="6">
+        <v>28</v>
+      </c>
+      <c r="H115" s="6">
+        <v>1</v>
+      </c>
+      <c r="I115" s="8">
+        <v>42859.593749999935</v>
+      </c>
+      <c r="J115">
+        <v>1.6215277777155279</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A116" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B116" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C116" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D116" s="6">
+        <v>1</v>
+      </c>
+      <c r="E116" s="6">
+        <v>4</v>
+      </c>
+      <c r="F116" s="6">
+        <v>5</v>
+      </c>
+      <c r="G116" s="6">
+        <v>29</v>
+      </c>
+      <c r="H116" s="6">
+        <v>1</v>
+      </c>
+      <c r="I116" s="8">
+        <v>42859.604166666599</v>
+      </c>
+      <c r="J116">
+        <v>1.6319444443797693</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A117" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B117" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C117" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D117" s="6">
+        <v>1</v>
+      </c>
+      <c r="E117" s="6">
+        <v>4</v>
+      </c>
+      <c r="F117" s="6">
+        <v>6</v>
+      </c>
+      <c r="G117" s="6">
+        <v>30</v>
+      </c>
+      <c r="H117" s="6">
+        <v>1</v>
+      </c>
+      <c r="I117" s="8">
+        <v>42859.614583333263</v>
+      </c>
+      <c r="J117">
+        <v>1.6423611110440106</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A118" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B118" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C118" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D118" s="6">
+        <v>1</v>
+      </c>
+      <c r="E118" s="6">
+        <v>4</v>
+      </c>
+      <c r="F118" s="6">
+        <v>7</v>
+      </c>
+      <c r="G118" s="6">
+        <v>31</v>
+      </c>
+      <c r="H118" s="6">
+        <v>1</v>
+      </c>
+      <c r="I118" s="8">
+        <v>42859.624999999927</v>
+      </c>
+      <c r="J118">
+        <v>1.652777777708252</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A119" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B119" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C119" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D119" s="6">
+        <v>1</v>
+      </c>
+      <c r="E119" s="6">
+        <v>4</v>
+      </c>
+      <c r="F119" s="6">
+        <v>8</v>
+      </c>
+      <c r="G119" s="6">
+        <v>32</v>
+      </c>
+      <c r="H119" s="6">
+        <v>1</v>
+      </c>
+      <c r="I119" s="8">
+        <v>42859.635416666591</v>
+      </c>
+      <c r="J119">
+        <v>1.6631944443724933</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A120" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B120" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C120" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D120" s="6">
+        <v>1</v>
+      </c>
+      <c r="E120" s="6">
+        <v>3</v>
+      </c>
+      <c r="F120" s="6">
+        <v>3</v>
+      </c>
+      <c r="G120" s="6">
+        <v>1</v>
+      </c>
+      <c r="H120" s="6">
+        <v>1</v>
+      </c>
+      <c r="I120" s="8">
+        <v>42859.645833333256</v>
+      </c>
+      <c r="J120">
+        <v>1.6736111110367347</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A121" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B121" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C121" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D121" s="6">
+        <v>1</v>
+      </c>
+      <c r="E121" s="6">
+        <v>3</v>
+      </c>
+      <c r="F121" s="6">
+        <v>4</v>
+      </c>
+      <c r="G121" s="6">
+        <v>2</v>
+      </c>
+      <c r="H121" s="6">
+        <v>1</v>
+      </c>
+      <c r="I121" s="8">
+        <v>42859.65624999992</v>
+      </c>
+      <c r="J121">
+        <v>1.684027777700976</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A122" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B122" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C122" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D122" s="6">
+        <v>1</v>
+      </c>
+      <c r="E122" s="6">
+        <v>3</v>
+      </c>
+      <c r="F122" s="6">
+        <v>5</v>
+      </c>
+      <c r="G122" s="6">
+        <v>3</v>
+      </c>
+      <c r="H122" s="6">
+        <v>1</v>
+      </c>
+      <c r="I122" s="8">
+        <v>42859.666666666584</v>
+      </c>
+      <c r="J122">
+        <v>1.6944444443652174</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A123" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B123" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C123" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D123" s="6">
+        <v>1</v>
+      </c>
+      <c r="E123" s="6">
+        <v>3</v>
+      </c>
+      <c r="F123" s="6">
+        <v>6</v>
+      </c>
+      <c r="G123" s="6">
+        <v>4</v>
+      </c>
+      <c r="H123" s="6">
+        <v>1</v>
+      </c>
+      <c r="I123" s="8">
+        <v>42859.677083333248</v>
+      </c>
+      <c r="J123">
+        <v>1.7048611110294587</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A124" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B124" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C124" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D124" s="6">
+        <v>1</v>
+      </c>
+      <c r="E124" s="6">
+        <v>3</v>
+      </c>
+      <c r="F124" s="6">
+        <v>7</v>
+      </c>
+      <c r="G124" s="6">
+        <v>5</v>
+      </c>
+      <c r="H124" s="6">
+        <v>1</v>
+      </c>
+      <c r="I124" s="8">
+        <v>42859.687499999913</v>
+      </c>
+      <c r="J124">
+        <v>1.7152777776937</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A125" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B125" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C125" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D125" s="6">
+        <v>1</v>
+      </c>
+      <c r="E125" s="6">
+        <v>3</v>
+      </c>
+      <c r="F125" s="6">
+        <v>8</v>
+      </c>
+      <c r="G125" s="6">
+        <v>6</v>
+      </c>
+      <c r="H125" s="6">
+        <v>1</v>
+      </c>
+      <c r="I125" s="8">
+        <v>42859.697916666577</v>
+      </c>
+      <c r="J125">
+        <v>1.7256944443579414</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A126" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B126" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C126" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D126" s="6">
+        <v>1</v>
+      </c>
+      <c r="E126" s="6">
+        <v>3</v>
+      </c>
+      <c r="F126" s="6">
+        <v>9</v>
+      </c>
+      <c r="G126" s="6">
+        <v>7</v>
+      </c>
+      <c r="H126" s="6">
+        <v>1</v>
+      </c>
+      <c r="I126" s="8">
+        <v>42859.708333333241</v>
+      </c>
+      <c r="J126">
+        <v>1.7361111110221827</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A127" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="B127" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C127" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D127" s="6">
+        <v>1</v>
+      </c>
+      <c r="E127" s="6">
+        <v>3</v>
+      </c>
+      <c r="F127" s="6">
+        <v>10</v>
+      </c>
+      <c r="G127" s="6">
+        <v>8</v>
+      </c>
+      <c r="H127" s="6">
+        <v>1</v>
+      </c>
+      <c r="I127" s="8">
+        <v>42859.718749999905</v>
+      </c>
+      <c r="J127">
+        <v>1.7465277776864241</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A128" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B128" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C128" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D128" s="6">
+        <v>1</v>
+      </c>
+      <c r="E128" s="6">
+        <v>4</v>
+      </c>
+      <c r="F128" s="6">
+        <v>3</v>
+      </c>
+      <c r="G128" s="6">
+        <v>9</v>
+      </c>
+      <c r="H128" s="6">
+        <v>1</v>
+      </c>
+      <c r="I128" s="8">
+        <v>42859.72916666657</v>
+      </c>
+      <c r="J128">
+        <v>1.7569444443506654</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A129" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B129" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C129" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D129" s="6">
+        <v>1</v>
+      </c>
+      <c r="E129" s="6">
+        <v>4</v>
+      </c>
+      <c r="F129" s="6">
+        <v>4</v>
+      </c>
+      <c r="G129" s="6">
+        <v>10</v>
+      </c>
+      <c r="H129" s="6">
+        <v>1</v>
+      </c>
+      <c r="I129" s="8">
+        <v>42859.739583333234</v>
+      </c>
+      <c r="J129">
+        <v>1.7673611110149068</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A130" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B130" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C130" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D130" s="6">
+        <v>1</v>
+      </c>
+      <c r="E130" s="6">
+        <v>4</v>
+      </c>
+      <c r="F130" s="6">
+        <v>5</v>
+      </c>
+      <c r="G130" s="6">
+        <v>11</v>
+      </c>
+      <c r="H130" s="6">
+        <v>1</v>
+      </c>
+      <c r="I130" s="8">
+        <v>42859.749999999898</v>
+      </c>
+      <c r="J130">
+        <v>1.7777777776791481</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A131" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="B131" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C131" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D131" s="6">
+        <v>1</v>
+      </c>
+      <c r="E131" s="6">
+        <v>4</v>
+      </c>
+      <c r="F131" s="6">
+        <v>6</v>
+      </c>
+      <c r="G131" s="6">
+        <v>12</v>
+      </c>
+      <c r="H131" s="6">
+        <v>1</v>
+      </c>
+      <c r="I131" s="8">
+        <v>42859.760416666562</v>
+      </c>
+      <c r="J131">
+        <v>1.7881944443433895</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A132" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B132" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C132" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D132" s="6">
+        <v>1</v>
+      </c>
+      <c r="E132" s="6">
+        <v>4</v>
+      </c>
+      <c r="F132" s="6">
+        <v>7</v>
+      </c>
+      <c r="G132" s="6">
+        <v>13</v>
+      </c>
+      <c r="H132" s="6">
+        <v>1</v>
+      </c>
+      <c r="I132" s="8">
+        <v>42859.770833333227</v>
+      </c>
+      <c r="J132">
+        <v>1.7986111110076308</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A133" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B133" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C133" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D133" s="6">
+        <v>1</v>
+      </c>
+      <c r="E133" s="6">
+        <v>4</v>
+      </c>
+      <c r="F133" s="6">
+        <v>8</v>
+      </c>
+      <c r="G133" s="6">
+        <v>14</v>
+      </c>
+      <c r="H133" s="6">
+        <v>1</v>
+      </c>
+      <c r="I133" s="8">
+        <v>42859.781249999891</v>
+      </c>
+      <c r="J133">
+        <v>1.8090277776718722</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A134" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="B134" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C134" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D134" s="6">
+        <v>1</v>
+      </c>
+      <c r="E134" s="6">
+        <v>4</v>
+      </c>
+      <c r="F134" s="6">
+        <v>9</v>
+      </c>
+      <c r="G134" s="6">
+        <v>15</v>
+      </c>
+      <c r="H134" s="6">
+        <v>1</v>
+      </c>
+      <c r="I134" s="8">
+        <v>42859.791666666555</v>
+      </c>
+      <c r="J134">
+        <v>1.8194444443361135</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A135" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B135" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C135" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D135" s="6">
+        <v>1</v>
+      </c>
+      <c r="E135" s="6">
+        <v>4</v>
+      </c>
+      <c r="F135" s="6">
+        <v>10</v>
+      </c>
+      <c r="G135" s="6">
+        <v>16</v>
+      </c>
+      <c r="H135" s="6">
+        <v>1</v>
+      </c>
+      <c r="I135" s="8">
+        <v>42859.802083333219</v>
+      </c>
+      <c r="J135">
+        <v>1.8298611110003549</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A136" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B136" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C136" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D136" s="6">
+        <v>1</v>
+      </c>
+      <c r="E136" s="6">
+        <v>5</v>
+      </c>
+      <c r="F136" s="6">
+        <v>3</v>
+      </c>
+      <c r="G136" s="6">
+        <v>17</v>
+      </c>
+      <c r="H136" s="6">
+        <v>1</v>
+      </c>
+      <c r="I136" s="8">
+        <v>42859.812499999884</v>
+      </c>
+      <c r="J136">
+        <v>1.8402777776645962</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A137" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="B137" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C137" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D137" s="6">
+        <v>1</v>
+      </c>
+      <c r="E137" s="6">
+        <v>5</v>
+      </c>
+      <c r="F137" s="6">
+        <v>4</v>
+      </c>
+      <c r="G137" s="6">
+        <v>18</v>
+      </c>
+      <c r="H137" s="6">
+        <v>1</v>
+      </c>
+      <c r="I137" s="8">
+        <v>42859.822916666548</v>
+      </c>
+      <c r="J137">
+        <v>1.8506944443288376</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A138" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B138" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C138" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D138" s="6">
+        <v>1</v>
+      </c>
+      <c r="E138" s="6">
+        <v>3</v>
+      </c>
+      <c r="F138" s="6">
+        <v>3</v>
+      </c>
+      <c r="G138" s="6">
+        <v>19</v>
+      </c>
+      <c r="H138" s="6">
+        <v>1</v>
+      </c>
+      <c r="I138" s="8">
+        <v>42859.833333333212</v>
+      </c>
+      <c r="J138">
+        <v>1.8611111109930789</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A139" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B139" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C139" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D139" s="6">
+        <v>1</v>
+      </c>
+      <c r="E139" s="6">
+        <v>3</v>
+      </c>
+      <c r="F139" s="6">
+        <v>4</v>
+      </c>
+      <c r="G139" s="6">
+        <v>20</v>
+      </c>
+      <c r="H139" s="6">
+        <v>1</v>
+      </c>
+      <c r="I139" s="8">
+        <v>42859.843749999876</v>
+      </c>
+      <c r="J139">
+        <v>1.8715277776573203</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A140" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="B140" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C140" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D140" s="6">
+        <v>1</v>
+      </c>
+      <c r="E140" s="6">
+        <v>3</v>
+      </c>
+      <c r="F140" s="6">
+        <v>5</v>
+      </c>
+      <c r="G140" s="6">
+        <v>21</v>
+      </c>
+      <c r="H140" s="6">
+        <v>1</v>
+      </c>
+      <c r="I140" s="8">
+        <v>42859.854166666541</v>
+      </c>
+      <c r="J140">
+        <v>1.8819444443215616</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A141" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="B141" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C141" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D141" s="6">
+        <v>1</v>
+      </c>
+      <c r="E141" s="6">
+        <v>3</v>
+      </c>
+      <c r="F141" s="6">
+        <v>6</v>
+      </c>
+      <c r="G141" s="6">
+        <v>22</v>
+      </c>
+      <c r="H141" s="6">
+        <v>1</v>
+      </c>
+      <c r="I141" s="8">
+        <v>42859.864583333205</v>
+      </c>
+      <c r="J141">
+        <v>1.892361110985803</v>
+      </c>
+    </row>
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A142" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B142" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C142" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D142" s="6">
+        <v>1</v>
+      </c>
+      <c r="E142" s="6">
+        <v>3</v>
+      </c>
+      <c r="F142" s="6">
+        <v>7</v>
+      </c>
+      <c r="G142" s="6">
+        <v>23</v>
+      </c>
+      <c r="H142" s="6">
+        <v>1</v>
+      </c>
+      <c r="I142" s="8">
+        <v>42859.874999999869</v>
+      </c>
+      <c r="J142">
+        <v>1.9027777776500443</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A143" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="B143" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C143" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D143" s="6">
+        <v>1</v>
+      </c>
+      <c r="E143" s="6">
+        <v>3</v>
+      </c>
+      <c r="F143" s="6">
+        <v>8</v>
+      </c>
+      <c r="G143" s="6">
+        <v>24</v>
+      </c>
+      <c r="H143" s="6">
+        <v>1</v>
+      </c>
+      <c r="I143" s="8">
+        <v>42859.885416666533</v>
+      </c>
+      <c r="J143">
+        <v>1.9131944443142856</v>
+      </c>
+    </row>
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A144" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="B144" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C144" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D144" s="6">
+        <v>1</v>
+      </c>
+      <c r="E144" s="6">
+        <v>3</v>
+      </c>
+      <c r="F144" s="6">
+        <v>9</v>
+      </c>
+      <c r="G144" s="6">
+        <v>25</v>
+      </c>
+      <c r="H144" s="6">
+        <v>1</v>
+      </c>
+      <c r="I144" s="8">
+        <v>42859.895833333198</v>
+      </c>
+      <c r="J144">
+        <v>1.923611110978527</v>
+      </c>
+    </row>
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A145" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B145" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C145" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D145" s="6">
+        <v>1</v>
+      </c>
+      <c r="E145" s="6">
+        <v>3</v>
+      </c>
+      <c r="F145" s="6">
+        <v>10</v>
+      </c>
+      <c r="G145" s="6">
+        <v>26</v>
+      </c>
+      <c r="H145" s="6">
+        <v>1</v>
+      </c>
+      <c r="I145" s="8">
+        <v>42859.906249999862</v>
+      </c>
+      <c r="J145">
+        <v>1.9340277776427683</v>
+      </c>
+    </row>
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A146" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="B146" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C146" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D146" s="6">
+        <v>1</v>
+      </c>
+      <c r="E146" s="6">
+        <v>4</v>
+      </c>
+      <c r="F146" s="6">
+        <v>3</v>
+      </c>
+      <c r="G146" s="6">
+        <v>27</v>
+      </c>
+      <c r="H146" s="6">
+        <v>1</v>
+      </c>
+      <c r="I146" s="8">
+        <v>42859.916666666526</v>
+      </c>
+      <c r="J146">
+        <v>1.9444444443070097</v>
+      </c>
+    </row>
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A147" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="B147" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C147" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D147" s="6">
+        <v>1</v>
+      </c>
+      <c r="E147" s="6">
+        <v>4</v>
+      </c>
+      <c r="F147" s="6">
+        <v>4</v>
+      </c>
+      <c r="G147" s="6">
+        <v>28</v>
+      </c>
+      <c r="H147" s="6">
+        <v>1</v>
+      </c>
+      <c r="I147" s="8">
+        <v>42859.92708333319</v>
+      </c>
+      <c r="J147">
+        <v>1.954861110971251</v>
+      </c>
+    </row>
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A148" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="B148" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C148" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D148" s="6">
+        <v>1</v>
+      </c>
+      <c r="E148" s="6">
+        <v>4</v>
+      </c>
+      <c r="F148" s="6">
+        <v>5</v>
+      </c>
+      <c r="G148" s="6">
+        <v>29</v>
+      </c>
+      <c r="H148" s="6">
+        <v>1</v>
+      </c>
+      <c r="I148" s="8">
+        <v>42859.937499999854</v>
+      </c>
+      <c r="J148">
+        <v>1.9652777776354924</v>
+      </c>
+    </row>
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A149" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="B149" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C149" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D149" s="6">
+        <v>1</v>
+      </c>
+      <c r="E149" s="6">
+        <v>4</v>
+      </c>
+      <c r="F149" s="6">
+        <v>6</v>
+      </c>
+      <c r="G149" s="6">
+        <v>30</v>
+      </c>
+      <c r="H149" s="6">
+        <v>1</v>
+      </c>
+      <c r="I149" s="8">
+        <v>42859.947916666519</v>
+      </c>
+      <c r="J149">
+        <v>1.9756944442997337</v>
+      </c>
+    </row>
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A150" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="B150" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C150" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D150" s="6">
+        <v>1</v>
+      </c>
+      <c r="E150" s="6">
+        <v>4</v>
+      </c>
+      <c r="F150" s="6">
+        <v>7</v>
+      </c>
+      <c r="G150" s="6">
+        <v>31</v>
+      </c>
+      <c r="H150" s="6">
+        <v>1</v>
+      </c>
+      <c r="I150" s="8">
+        <v>42859.958333333183</v>
+      </c>
+      <c r="J150">
+        <v>1.9861111109639751</v>
+      </c>
+    </row>
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A151" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="B151" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C151" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D151" s="6">
+        <v>1</v>
+      </c>
+      <c r="E151" s="6">
+        <v>4</v>
+      </c>
+      <c r="F151" s="6">
+        <v>8</v>
+      </c>
+      <c r="G151" s="6">
+        <v>32</v>
+      </c>
+      <c r="H151" s="6">
+        <v>1</v>
+      </c>
+      <c r="I151" s="8">
+        <v>42859.968749999847</v>
+      </c>
+      <c r="J151">
+        <v>1.9965277776282164</v>
+      </c>
+    </row>
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A152" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="B152" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C152" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D152" s="6">
+        <v>1</v>
+      </c>
+      <c r="E152" s="6">
+        <v>3</v>
+      </c>
+      <c r="F152" s="6">
+        <v>3</v>
+      </c>
+      <c r="G152" s="6">
+        <v>1</v>
+      </c>
+      <c r="H152" s="6">
+        <v>1</v>
+      </c>
+      <c r="I152" s="8">
+        <v>42859.979166666511</v>
+      </c>
+      <c r="J152">
+        <v>2.0069444442924578</v>
+      </c>
+    </row>
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A153" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="B153" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C153" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D153" s="6">
+        <v>1</v>
+      </c>
+      <c r="E153" s="6">
+        <v>3</v>
+      </c>
+      <c r="F153" s="6">
+        <v>4</v>
+      </c>
+      <c r="G153" s="6">
+        <v>2</v>
+      </c>
+      <c r="H153" s="6">
+        <v>1</v>
+      </c>
+      <c r="I153" s="8">
+        <v>42859.989583333176</v>
+      </c>
+      <c r="J153">
+        <v>2.0173611109566991</v>
+      </c>
+    </row>
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A154" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="B154" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C154" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D154" s="6">
+        <v>1</v>
+      </c>
+      <c r="E154" s="6">
+        <v>3</v>
+      </c>
+      <c r="F154" s="6">
+        <v>5</v>
+      </c>
+      <c r="G154" s="6">
+        <v>3</v>
+      </c>
+      <c r="H154" s="6">
+        <v>1</v>
+      </c>
+      <c r="I154" s="8">
+        <v>42859.99999999984</v>
+      </c>
+      <c r="J154">
+        <v>2.0277777776209405</v>
+      </c>
+    </row>
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A155" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="B155" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C155" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D155" s="6">
+        <v>1</v>
+      </c>
+      <c r="E155" s="6">
+        <v>3</v>
+      </c>
+      <c r="F155" s="6">
+        <v>6</v>
+      </c>
+      <c r="G155" s="6">
+        <v>4</v>
+      </c>
+      <c r="H155" s="6">
+        <v>1</v>
+      </c>
+      <c r="I155" s="8">
+        <v>42860.010416666504</v>
+      </c>
+      <c r="J155">
+        <v>2.0381944442851818</v>
+      </c>
+    </row>
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A156" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="B156" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C156" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D156" s="6">
+        <v>1</v>
+      </c>
+      <c r="E156" s="6">
+        <v>3</v>
+      </c>
+      <c r="F156" s="6">
+        <v>7</v>
+      </c>
+      <c r="G156" s="6">
+        <v>5</v>
+      </c>
+      <c r="H156" s="6">
+        <v>1</v>
+      </c>
+      <c r="I156" s="8">
+        <v>42860.020833333168</v>
+      </c>
+      <c r="J156">
+        <v>2.0486111109494232</v>
+      </c>
+    </row>
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A157" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="B157" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C157" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D157" s="6">
+        <v>1</v>
+      </c>
+      <c r="E157" s="6">
+        <v>3</v>
+      </c>
+      <c r="F157" s="6">
+        <v>8</v>
+      </c>
+      <c r="G157" s="6">
+        <v>6</v>
+      </c>
+      <c r="H157" s="6">
+        <v>1</v>
+      </c>
+      <c r="I157" s="8">
+        <v>42860.031249999833</v>
+      </c>
+      <c r="J157">
+        <v>2.0590277776136645</v>
+      </c>
+    </row>
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A158" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="B158" s="7">
+        <v>42857.972222222219</v>
+      </c>
+      <c r="C158" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D158" s="6">
+        <v>1</v>
+      </c>
+      <c r="E158" s="6">
+        <v>3</v>
+      </c>
+      <c r="F158" s="6">
+        <v>9</v>
+      </c>
+      <c r="G158" s="6">
+        <v>7</v>
+      </c>
+      <c r="H158" s="6">
+        <v>1</v>
+      </c>
+      <c r="I158" s="8">
+        <v>42860.041666666497</v>
+      </c>
+      <c r="J158">
+        <v>2.0694444442779059</v>
+      </c>
+    </row>
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D159" s="6"/>
+      <c r="E159" s="6"/>
+      <c r="F159" s="6"/>
+      <c r="G159" s="6"/>
+      <c r="H159" s="6"/>
+    </row>
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D160" s="6"/>
+      <c r="E160" s="6"/>
+      <c r="F160" s="6"/>
+      <c r="G160" s="6"/>
+      <c r="H160" s="6"/>
+    </row>
+    <row r="161" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D161" s="6"/>
+      <c r="E161" s="6"/>
+      <c r="F161" s="6"/>
+      <c r="G161" s="6"/>
+      <c r="H161" s="6"/>
+    </row>
+    <row r="162" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D162" s="6"/>
+      <c r="E162" s="6"/>
+      <c r="F162" s="6"/>
+      <c r="G162" s="6"/>
+      <c r="H162" s="6"/>
+    </row>
+    <row r="163" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D163" s="6"/>
+      <c r="E163" s="6"/>
+      <c r="F163" s="6"/>
+      <c r="G163" s="6"/>
+      <c r="H163" s="6"/>
+    </row>
+    <row r="164" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D164" s="6"/>
+      <c r="E164" s="6"/>
+      <c r="F164" s="6"/>
+      <c r="G164" s="6"/>
+      <c r="H164" s="6"/>
+    </row>
+    <row r="165" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D165" s="6"/>
+      <c r="E165" s="6"/>
+      <c r="F165" s="6"/>
+      <c r="G165" s="6"/>
+      <c r="H165" s="6"/>
+    </row>
+    <row r="166" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D166" s="6"/>
+      <c r="E166" s="6"/>
+      <c r="F166" s="6"/>
+      <c r="G166" s="6"/>
+      <c r="H166" s="6"/>
+    </row>
+    <row r="167" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D167" s="6"/>
+      <c r="E167" s="6"/>
+      <c r="F167" s="6"/>
+      <c r="G167" s="6"/>
+      <c r="H167" s="6"/>
+    </row>
+    <row r="168" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D168" s="6"/>
+      <c r="E168" s="6"/>
+      <c r="F168" s="6"/>
+      <c r="G168" s="6"/>
+      <c r="H168" s="6"/>
+    </row>
+    <row r="169" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D169" s="6"/>
+      <c r="E169" s="6"/>
+      <c r="F169" s="6"/>
+      <c r="G169" s="6"/>
+      <c r="H169" s="6"/>
+    </row>
+    <row r="170" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D170" s="6"/>
+      <c r="E170" s="6"/>
+      <c r="F170" s="6"/>
+      <c r="G170" s="6"/>
+      <c r="H170" s="6"/>
+    </row>
+    <row r="171" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D171" s="6"/>
+      <c r="E171" s="6"/>
+      <c r="F171" s="6"/>
+      <c r="G171" s="6"/>
+      <c r="H171" s="6"/>
+    </row>
+    <row r="172" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D172" s="6"/>
+      <c r="E172" s="6"/>
+      <c r="F172" s="6"/>
+      <c r="G172" s="6"/>
+      <c r="H172" s="6"/>
+    </row>
+    <row r="173" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D173" s="6"/>
+      <c r="E173" s="6"/>
+      <c r="F173" s="6"/>
+      <c r="G173" s="6"/>
+      <c r="H173" s="6"/>
+    </row>
+    <row r="174" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D174" s="6"/>
+      <c r="E174" s="6"/>
+      <c r="F174" s="6"/>
+      <c r="G174" s="6"/>
+      <c r="H174" s="6"/>
+    </row>
+    <row r="175" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D175" s="6"/>
+      <c r="E175" s="6"/>
+      <c r="F175" s="6"/>
+      <c r="G175" s="6"/>
+      <c r="H175" s="6"/>
+    </row>
+    <row r="176" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D176" s="6"/>
+      <c r="E176" s="6"/>
+      <c r="F176" s="6"/>
+      <c r="G176" s="6"/>
+      <c r="H176" s="6"/>
+    </row>
+    <row r="177" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D177" s="6"/>
+      <c r="E177" s="6"/>
+      <c r="F177" s="6"/>
+      <c r="G177" s="6"/>
+      <c r="H177" s="6"/>
+    </row>
+    <row r="178" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D178" s="6"/>
+      <c r="E178" s="6"/>
+      <c r="F178" s="6"/>
+      <c r="G178" s="6"/>
+      <c r="H178" s="6"/>
+    </row>
+    <row r="179" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D179" s="6"/>
+      <c r="E179" s="6"/>
+      <c r="F179" s="6"/>
+      <c r="G179" s="6"/>
+      <c r="H179" s="6"/>
+    </row>
+    <row r="180" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D180" s="6"/>
+      <c r="E180" s="6"/>
+      <c r="F180" s="6"/>
+      <c r="G180" s="6"/>
+      <c r="H180" s="6"/>
+    </row>
+    <row r="181" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D181" s="6"/>
+      <c r="E181" s="6"/>
+      <c r="F181" s="6"/>
+      <c r="G181" s="6"/>
+      <c r="H181" s="6"/>
+    </row>
+    <row r="182" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D182" s="6"/>
+      <c r="E182" s="6"/>
+      <c r="F182" s="6"/>
+      <c r="G182" s="6"/>
+      <c r="H182" s="6"/>
+    </row>
+    <row r="183" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D183" s="6"/>
+      <c r="E183" s="6"/>
+      <c r="F183" s="6"/>
+      <c r="G183" s="6"/>
+      <c r="H183" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>